<commit_message>
melhoria de gráficos e organização das bases
</commit_message>
<xml_diff>
--- a/salvo_excel/saldo_porto_maranhao.xlsx
+++ b/salvo_excel/saldo_porto_maranhao.xlsx
@@ -392,7 +392,7 @@
         <v>202002</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -405,7 +405,7 @@
         <v>202003</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-67</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -418,7 +418,7 @@
         <v>202004</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>-111</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -431,7 +431,7 @@
         <v>202005</v>
       </c>
       <c r="B6">
-        <v>-9</v>
+        <v>-108</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -444,7 +444,7 @@
         <v>202006</v>
       </c>
       <c r="B7">
-        <v>-12</v>
+        <v>-40</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -457,7 +457,7 @@
         <v>202007</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -470,7 +470,7 @@
         <v>202008</v>
       </c>
       <c r="B9">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -483,7 +483,7 @@
         <v>202009</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -496,7 +496,7 @@
         <v>202010</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
         <v>202011</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         <v>202012</v>
       </c>
       <c r="B13">
-        <v>-3</v>
+        <v>-18</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -535,7 +535,7 @@
         <v>202101</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
         <v>202102</v>
       </c>
       <c r="B15">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -561,7 +561,7 @@
         <v>202103</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>-8</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -574,7 +574,7 @@
         <v>202104</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -587,7 +587,7 @@
         <v>202105</v>
       </c>
       <c r="B18">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         <v>202106</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -613,7 +613,7 @@
         <v>202107</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
         <v>202108</v>
       </c>
       <c r="B21">
-        <v>-2</v>
+        <v>59</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         <v>202109</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
         <v>202110</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -665,7 +665,7 @@
         <v>202111</v>
       </c>
       <c r="B24">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         <v>202112</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>-31</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         <v>202201</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -704,7 +704,7 @@
         <v>202202</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>202203</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         <v>202204</v>
       </c>
       <c r="B29">
-        <v>-10</v>
+        <v>109</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -743,7 +743,7 @@
         <v>202205</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
         <v>202206</v>
       </c>
       <c r="B31">
-        <v>-6</v>
+        <v>48</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         <v>202207</v>
       </c>
       <c r="B32">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         <v>202208</v>
       </c>
       <c r="B33">
-        <v>-5</v>
+        <v>128</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
         <v>202209</v>
       </c>
       <c r="B34">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -808,7 +808,7 @@
         <v>202210</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -821,7 +821,7 @@
         <v>202211</v>
       </c>
       <c r="B36">
-        <v>27</v>
+        <v>201</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         <v>202212</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>-19</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         <v>202301</v>
       </c>
       <c r="B38">
-        <v>-9</v>
+        <v>60</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
         <v>202302</v>
       </c>
       <c r="B39">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
         <v>202303</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -886,7 +886,7 @@
         <v>202304</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -899,7 +899,7 @@
         <v>202305</v>
       </c>
       <c r="B42">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
         <v>202306</v>
       </c>
       <c r="B43">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         <v>202307</v>
       </c>
       <c r="B44">
-        <v>-4</v>
+        <v>23</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -938,7 +938,7 @@
         <v>202308</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>-67</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
         <v>202309</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>202310</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -977,7 +977,7 @@
         <v>202311</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
         <v>202312</v>
       </c>
       <c r="B49">
-        <v>-5</v>
+        <v>-40</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>